<commit_message>
Adicionado mapa do Desert Resort
</commit_message>
<xml_diff>
--- a/other/Encounter locations.xlsx
+++ b/other/Encounter locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526C962C-221E-4E2F-893D-67AF7E970BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B580CC0-BEBC-45F9-8A10-B724D1B82C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,14 +756,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -781,6 +778,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1153,7 +1153,7 @@
   <dimension ref="B1:P62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,34 +1175,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="16"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="19"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -1220,21 +1220,21 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="11" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="J4" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
       <c r="O4" t="s">
         <v>80</v>
       </c>
@@ -1685,12 +1685,12 @@
       <c r="H16" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
       <c r="O16" t="s">
         <v>92</v>
       </c>
@@ -2637,7 +2637,7 @@
       <c r="C45" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="12">
+      <c r="D45" s="10">
         <v>0.2</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -2964,7 +2964,7 @@
       <c r="E60" t="s">
         <v>161</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F60" s="11" t="s">
         <v>160</v>
       </c>
       <c r="G60" t="s">

</xml_diff>

<commit_message>
Mapa do relic castle atualizado e correções de bugs
</commit_message>
<xml_diff>
--- a/other/Encounter locations.xlsx
+++ b/other/Encounter locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B580CC0-BEBC-45F9-8A10-B724D1B82C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E85B6A-3D39-40C2-865E-151A77D10118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="175">
   <si>
     <t>Pokemon</t>
   </si>
@@ -548,6 +548,18 @@
   </si>
   <si>
     <t>Castelia Stove</t>
+  </si>
+  <si>
+    <t>Sneasel</t>
+  </si>
+  <si>
+    <t>Gible</t>
+  </si>
+  <si>
+    <t>Pansage</t>
+  </si>
+  <si>
+    <t>Pansear</t>
   </si>
 </sst>
 </file>
@@ -835,8 +847,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H62" totalsRowShown="0">
-  <autoFilter ref="B5:H62" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H67" totalsRowShown="0">
+  <autoFilter ref="B5:H67" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CCB72512-45BE-4582-B5B1-F7A9C3F7785B}" name="Pokemon"/>
     <tableColumn id="2" xr3:uid="{2758C6CC-A2DA-4CFB-B52E-6AE39BDC339C}" name="Location"/>
@@ -1150,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P62"/>
+  <dimension ref="B1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1409,7 @@
         <v>84</v>
       </c>
       <c r="P8">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
@@ -1590,7 +1602,7 @@
         <v>89</v>
       </c>
       <c r="P13">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -1631,7 +1643,7 @@
         <v>90</v>
       </c>
       <c r="P14">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
@@ -1660,30 +1672,30 @@
         <v>91</v>
       </c>
       <c r="P15">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="D16" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
         <v>160</v>
       </c>
       <c r="G16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" t="s">
         <v>72</v>
-      </c>
-      <c r="H16" t="s">
-        <v>47</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>110</v>
@@ -1700,21 +1712,24 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="D17" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E17" t="s">
         <v>161</v>
       </c>
       <c r="F17" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" t="s">
         <v>47</v>
       </c>
       <c r="J17" t="s">
@@ -1738,10 +1753,10 @@
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D18" s="5">
         <v>0.05</v>
@@ -1750,13 +1765,10 @@
         <v>161</v>
       </c>
       <c r="F18" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J18" t="s">
         <v>35</v>
@@ -1774,30 +1786,30 @@
         <v>94</v>
       </c>
       <c r="P18">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>13</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="D19" s="5">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J19" t="s">
         <v>114</v>
@@ -1815,30 +1827,30 @@
         <v>95</v>
       </c>
       <c r="P19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="5">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
@@ -1856,18 +1868,18 @@
         <v>96</v>
       </c>
       <c r="P20">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="D21" s="5">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E21" t="s">
         <v>161</v>
@@ -1876,10 +1888,10 @@
         <v>160</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="J21" t="s">
         <v>30</v>
@@ -1902,13 +1914,13 @@
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="C22" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D22" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E22" t="s">
         <v>161</v>
@@ -1917,7 +1929,10 @@
         <v>160</v>
       </c>
       <c r="G22" t="s">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="H22" t="s">
+        <v>76</v>
       </c>
       <c r="J22" t="s">
         <v>31</v>
@@ -1934,25 +1949,22 @@
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="D23" s="5">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E23" t="s">
         <v>161</v>
       </c>
       <c r="F23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J23" t="s">
         <v>32</v>
@@ -1966,25 +1978,25 @@
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="C24" t="s">
         <v>129</v>
       </c>
       <c r="D24" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E24" t="s">
         <v>161</v>
       </c>
       <c r="F24" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G24" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J24" t="s">
         <v>28</v>
@@ -2001,22 +2013,22 @@
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="D25" s="5">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="F25" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H25" t="s">
         <v>53</v>
@@ -2033,25 +2045,25 @@
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="D26" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E26" t="s">
-        <v>161</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
         <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="J26" t="s">
         <v>37</v>
@@ -2068,10 +2080,10 @@
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D27" s="5">
         <v>0.2</v>
@@ -2083,10 +2095,10 @@
         <v>160</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="H27" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="J27" t="s">
         <v>59</v>
@@ -2103,22 +2115,25 @@
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="D28" s="5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E28" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F28" t="s">
         <v>160</v>
       </c>
       <c r="G28" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="H28" t="s">
+        <v>58</v>
       </c>
       <c r="J28" t="s">
         <v>98</v>
@@ -2132,16 +2147,16 @@
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="5">
-        <v>0.17</v>
+        <v>0.3</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>168</v>
       </c>
       <c r="F29" t="s">
         <v>160</v>
@@ -2149,9 +2164,6 @@
       <c r="G29" t="s">
         <v>50</v>
       </c>
-      <c r="H29" t="s">
-        <v>48</v>
-      </c>
       <c r="J29" t="s">
         <v>99</v>
       </c>
@@ -2167,16 +2179,16 @@
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>146</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="5">
-        <v>0.3</v>
+        <v>0.17</v>
       </c>
       <c r="E30" t="s">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="F30" t="s">
         <v>160</v>
@@ -2184,6 +2196,9 @@
       <c r="G30" t="s">
         <v>50</v>
       </c>
+      <c r="H30" t="s">
+        <v>48</v>
+      </c>
       <c r="J30" t="s">
         <v>100</v>
       </c>
@@ -2199,25 +2214,22 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C31" t="s">
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="D31" s="5">
-        <v>0.01</v>
+        <v>0.3</v>
       </c>
       <c r="E31" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F31" t="s">
         <v>160</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="J31" t="s">
         <v>101</v>
@@ -2234,13 +2246,13 @@
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="D32" s="5">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E32" t="s">
         <v>161</v>
@@ -2249,7 +2261,10 @@
         <v>160</v>
       </c>
       <c r="G32" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="H32" t="s">
+        <v>76</v>
       </c>
       <c r="J32" t="s">
         <v>102</v>
@@ -2266,13 +2281,13 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="5">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E33" t="s">
         <v>161</v>
@@ -2281,10 +2296,7 @@
         <v>160</v>
       </c>
       <c r="G33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J33" t="s">
         <v>103</v>
@@ -2298,21 +2310,24 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="C34" t="s">
         <v>129</v>
       </c>
       <c r="D34" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F34" t="s">
         <v>160</v>
       </c>
       <c r="G34" t="s">
+        <v>126</v>
+      </c>
+      <c r="H34" t="s">
         <v>47</v>
       </c>
       <c r="J34" t="s">
@@ -2330,25 +2345,25 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="5">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F35" t="s">
         <v>160</v>
       </c>
       <c r="G35" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J35" t="s">
         <v>105</v>
@@ -2362,10 +2377,10 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>23</v>
+        <v>145</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D36" s="5">
         <v>0.1</v>
@@ -2377,10 +2392,7 @@
         <v>160</v>
       </c>
       <c r="G36" t="s">
-        <v>45</v>
-      </c>
-      <c r="H36" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J36" t="s">
         <v>106</v>
@@ -2397,10 +2409,10 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>44</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
@@ -2412,7 +2424,10 @@
         <v>160</v>
       </c>
       <c r="G37" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="H37" t="s">
+        <v>53</v>
       </c>
       <c r="J37" t="s">
         <v>107</v>
@@ -2429,22 +2444,22 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D38" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F38" t="s">
         <v>160</v>
       </c>
       <c r="G38" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H38" t="s">
         <v>55</v>
@@ -2461,7 +2476,7 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
         <v>170</v>
@@ -2476,7 +2491,7 @@
         <v>160</v>
       </c>
       <c r="G39" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J39" t="s">
         <v>109</v>
@@ -2493,22 +2508,25 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>142</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D40" s="5">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F40" t="s">
         <v>160</v>
       </c>
       <c r="G40" t="s">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="H40" t="s">
+        <v>55</v>
       </c>
       <c r="J40" t="s">
         <v>41</v>
@@ -2525,22 +2543,22 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>143</v>
+        <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="D41" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F41" t="s">
         <v>160</v>
       </c>
       <c r="G41" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J41" t="s">
         <v>125</v>
@@ -2554,25 +2572,22 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D42" s="5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F42" t="s">
         <v>160</v>
       </c>
       <c r="G42" t="s">
-        <v>76</v>
-      </c>
-      <c r="H42" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J42" t="s">
         <v>124</v>
@@ -2589,79 +2604,67 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" t="s">
-        <v>44</v>
+        <v>174</v>
       </c>
       <c r="D43" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F43" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G43" t="s">
-        <v>47</v>
-      </c>
-      <c r="H43" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D44" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F44" t="s">
         <v>160</v>
       </c>
       <c r="G44" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D45" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>53</v>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E45" t="s">
+        <v>161</v>
+      </c>
+      <c r="F45" t="s">
+        <v>160</v>
+      </c>
+      <c r="G45" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C46" t="s">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="D46" s="5">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="E46" t="s">
         <v>161</v>
@@ -2670,21 +2673,18 @@
         <v>160</v>
       </c>
       <c r="G46" t="s">
-        <v>56</v>
-      </c>
-      <c r="H46" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="D47" s="5">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E47" t="s">
         <v>161</v>
@@ -2693,81 +2693,87 @@
         <v>160</v>
       </c>
       <c r="G47" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="H47" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="D48" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E48" t="s">
         <v>161</v>
       </c>
       <c r="F48" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G48" t="s">
-        <v>116</v>
+        <v>47</v>
       </c>
       <c r="H48" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D49" s="5">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E49" t="s">
         <v>161</v>
       </c>
       <c r="F49" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G49" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" t="s">
-        <v>165</v>
-      </c>
-      <c r="D50" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="E50" t="s">
-        <v>161</v>
-      </c>
-      <c r="F50" t="s">
-        <v>160</v>
-      </c>
-      <c r="G50" t="s">
-        <v>58</v>
+      <c r="B50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D50" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>38</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D51" s="5">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E51" t="s">
         <v>161</v>
@@ -2776,18 +2782,21 @@
         <v>160</v>
       </c>
       <c r="G51" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+      <c r="H51" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="C52" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="D52" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E52" t="s">
         <v>161</v>
@@ -2796,18 +2805,18 @@
         <v>160</v>
       </c>
       <c r="G52" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="D53" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E53" t="s">
         <v>161</v>
@@ -2816,27 +2825,27 @@
         <v>160</v>
       </c>
       <c r="G53" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="H53" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C54" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D54" s="5">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E54" t="s">
         <v>161</v>
       </c>
       <c r="F54" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G54" t="s">
         <v>76</v>
@@ -2844,13 +2853,13 @@
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>135</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D55" s="5">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
       <c r="E55" t="s">
         <v>161</v>
@@ -2859,18 +2868,18 @@
         <v>160</v>
       </c>
       <c r="G55" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>136</v>
+        <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D56" s="5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E56" t="s">
         <v>161</v>
@@ -2879,18 +2888,18 @@
         <v>160</v>
       </c>
       <c r="G56" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="D57" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E57" t="s">
         <v>161</v>
@@ -2899,21 +2908,18 @@
         <v>160</v>
       </c>
       <c r="G57" t="s">
-        <v>57</v>
-      </c>
-      <c r="H57" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>138</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
         <v>44</v>
       </c>
       <c r="D58" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E58" t="s">
         <v>161</v>
@@ -2922,49 +2928,46 @@
         <v>160</v>
       </c>
       <c r="G58" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H58" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="D59" s="5">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E59" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F59" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G59" t="s">
-        <v>60</v>
-      </c>
-      <c r="H59" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C60" t="s">
         <v>166</v>
       </c>
       <c r="D60" s="5">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="E60" t="s">
         <v>161</v>
       </c>
-      <c r="F60" s="11" t="s">
+      <c r="F60" t="s">
         <v>160</v>
       </c>
       <c r="G60" t="s">
@@ -2973,13 +2976,13 @@
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>113</v>
+        <v>166</v>
       </c>
       <c r="D61" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E61" t="s">
         <v>161</v>
@@ -2988,15 +2991,15 @@
         <v>160</v>
       </c>
       <c r="G61" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C62" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D62" s="5">
         <v>0.1</v>
@@ -3005,12 +3008,121 @@
         <v>161</v>
       </c>
       <c r="F62" t="s">
+        <v>160</v>
+      </c>
+      <c r="G62" t="s">
+        <v>57</v>
+      </c>
+      <c r="H62" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>161</v>
+      </c>
+      <c r="F63" t="s">
+        <v>160</v>
+      </c>
+      <c r="G63" t="s">
+        <v>53</v>
+      </c>
+      <c r="H63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="5">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>79</v>
+      </c>
+      <c r="F64" t="s">
         <v>163</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G64" t="s">
+        <v>60</v>
+      </c>
+      <c r="H64" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" t="s">
+        <v>166</v>
+      </c>
+      <c r="D65" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="E65" t="s">
+        <v>161</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>161</v>
+      </c>
+      <c r="F66" t="s">
+        <v>160</v>
+      </c>
+      <c r="G66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D67" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>161</v>
+      </c>
+      <c r="F67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G67" t="s">
         <v>47</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H67" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizada tabela com encounters
</commit_message>
<xml_diff>
--- a/other/Encounter locations.xlsx
+++ b/other/Encounter locations.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E85B6A-3D39-40C2-865E-151A77D10118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCA58E7-F81A-428E-AF3E-BBDA885A70F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Unova" sheetId="1" r:id="rId1"/>
+    <sheet name="Encounter locations" sheetId="1" r:id="rId1"/>
+    <sheet name="Types balancement" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="174">
   <si>
     <t>Pokemon</t>
   </si>
@@ -277,60 +278,6 @@
     <t>Static</t>
   </si>
   <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>fighting</t>
-  </si>
-  <si>
-    <t>flying</t>
-  </si>
-  <si>
-    <t>poison</t>
-  </si>
-  <si>
-    <t>ground</t>
-  </si>
-  <si>
-    <t>rock</t>
-  </si>
-  <si>
-    <t>bug</t>
-  </si>
-  <si>
-    <t>ghost</t>
-  </si>
-  <si>
-    <t>steel</t>
-  </si>
-  <si>
-    <t>fire</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>grass</t>
-  </si>
-  <si>
-    <t>electric</t>
-  </si>
-  <si>
-    <t>psychic</t>
-  </si>
-  <si>
-    <t>ice</t>
-  </si>
-  <si>
-    <t>dragon</t>
-  </si>
-  <si>
-    <t>dark</t>
-  </si>
-  <si>
-    <t>fairy</t>
-  </si>
-  <si>
     <t>Abra</t>
   </si>
   <si>
@@ -418,9 +365,6 @@
     <t>Dragon</t>
   </si>
   <si>
-    <t>Castelia Pokemon Center</t>
-  </si>
-  <si>
     <t>Nimbasa College</t>
   </si>
   <si>
@@ -560,13 +504,67 @@
   </si>
   <si>
     <t>Pansear</t>
+  </si>
+  <si>
+    <t>Castelia Pokemon Center (as a fossil)</t>
+  </si>
+  <si>
+    <t>Dex Types Balancement</t>
+  </si>
+  <si>
+    <t>Wingull</t>
+  </si>
+  <si>
+    <t>Aron</t>
+  </si>
+  <si>
+    <t>Torkoal</t>
+  </si>
+  <si>
+    <t>Lunatone</t>
+  </si>
+  <si>
+    <t>Solrock</t>
+  </si>
+  <si>
+    <t>Nihilego</t>
+  </si>
+  <si>
+    <t>Ultra Abyssmal Cave</t>
+  </si>
+  <si>
+    <t>Buzzwole</t>
+  </si>
+  <si>
+    <t>Pheromosa</t>
+  </si>
+  <si>
+    <t>Xurkitree</t>
+  </si>
+  <si>
+    <t>Celesteela</t>
+  </si>
+  <si>
+    <t>Kartana</t>
+  </si>
+  <si>
+    <t>Guzzlord</t>
+  </si>
+  <si>
+    <t>Poipole</t>
+  </si>
+  <si>
+    <t>Stakataka</t>
+  </si>
+  <si>
+    <t>Blacephalon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,6 +599,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -753,23 +759,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,11 +799,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -846,9 +872,1346 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Types balancement'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Amount</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-336A-4737-A50E-FDE2DE8E6010}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Types balancement'!$B$5:$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Normal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fighting</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flying</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Poison</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ground</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rock</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bug</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ghost</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Steel</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Fire</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Water</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Grass</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Electric</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Psychic</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Ice</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Dragon</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Dark</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Fairy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Types balancement'!$C$5:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C8E-48A5-9D9C-8CD7691C9D67}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>604470</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>181707</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>608134</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1290536-5A20-18AD-095F-D3BF64ED3B13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H67" totalsRowShown="0">
-  <autoFilter ref="B5:H67" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H82" totalsRowShown="0">
+  <autoFilter ref="B5:H82" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CCB72512-45BE-4582-B5B1-F7A9C3F7785B}" name="Pokemon"/>
     <tableColumn id="2" xr3:uid="{2758C6CC-A2DA-4CFB-B52E-6AE39BDC339C}" name="Location"/>
@@ -863,7 +2226,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3434D8B-BDAB-4ECD-8A85-C7E80B714D7A}" name="Tabela2" displayName="Tabela2" ref="J5:M14" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3434D8B-BDAB-4ECD-8A85-C7E80B714D7A}" name="Tabela2" displayName="Tabela2" ref="J5:M14" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="J5:M14" xr:uid="{A3434D8B-BDAB-4ECD-8A85-C7E80B714D7A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2BD04AA1-A54A-45BB-9100-8A6417A1B02F}" name="Pokemon"/>
@@ -876,17 +2239,6 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6D6978E1-009A-4781-8FD7-539D0DD98898}" name="Tabela3" displayName="Tabela3" ref="O3:P21" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="O3:P21" xr:uid="{6D6978E1-009A-4781-8FD7-539D0DD98898}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CD2085A3-1842-4985-9691-113AC6E69B92}" name="Type"/>
-    <tableColumn id="2" xr3:uid="{66919A9A-08A7-40FB-BEE4-263F90AD2D6D}" name="Amount"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{72A29798-ECB2-4617-83A6-C7BACCB91CB8}" name="Tabela4" displayName="Tabela4" ref="J17:M42" totalsRowShown="0">
   <autoFilter ref="J17:M42" xr:uid="{72A29798-ECB2-4617-83A6-C7BACCB91CB8}"/>
   <tableColumns count="4">
@@ -894,6 +2246,19 @@
     <tableColumn id="2" xr3:uid="{B2551E6E-006E-40DB-A0AC-0C5A314DF37D}" name="Location"/>
     <tableColumn id="3" xr3:uid="{3099F344-E0B9-4B13-9B2F-31066906E3AD}" name="Type 1"/>
     <tableColumn id="4" xr3:uid="{8A7D64A5-91CC-4EA1-9F12-F056E345B616}" name="Type 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6D6978E1-009A-4781-8FD7-539D0DD98898}" name="Tabela3" displayName="Tabela3" ref="B4:C22" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B4:C22" xr:uid="{6D6978E1-009A-4781-8FD7-539D0DD98898}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CD2085A3-1842-4985-9691-113AC6E69B92}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{DE8EF76B-40D8-4742-B62F-757C6B43A9D1}" name="Amount" dataDxfId="0">
+      <calculatedColumnFormula>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1162,16 +2527,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P67"/>
+  <dimension ref="B1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
@@ -1179,44 +2544,44 @@
     <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.85546875" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15"/>
-    </row>
-    <row r="2" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="18"/>
-    </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1224,37 +2589,25 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="O3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+    </row>
+    <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="J4" s="19" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="J4" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="O4" t="s">
-        <v>80</v>
-      </c>
-      <c r="P4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -1288,28 +2641,22 @@
       <c r="M5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O5" t="s">
-        <v>81</v>
-      </c>
-      <c r="P5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="D6" s="5">
         <v>0.1</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F6" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G6" t="s">
         <v>47</v>
@@ -1329,25 +2676,19 @@
       <c r="M6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="O6" t="s">
-        <v>82</v>
-      </c>
-      <c r="P6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="E7" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F7" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G7" t="s">
         <v>45</v>
@@ -1367,16 +2708,10 @@
       <c r="M7" t="s">
         <v>76</v>
       </c>
-      <c r="O7" t="s">
-        <v>83</v>
-      </c>
-      <c r="P7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
@@ -1385,10 +2720,10 @@
         <v>0.15</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F8" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="G8" t="s">
         <v>56</v>
@@ -1405,14 +2740,8 @@
       <c r="M8" t="s">
         <v>48</v>
       </c>
-      <c r="O8" t="s">
-        <v>84</v>
-      </c>
-      <c r="P8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1426,7 +2755,7 @@
         <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>48</v>
@@ -1446,28 +2775,22 @@
       <c r="M9" t="s">
         <v>53</v>
       </c>
-      <c r="O9" t="s">
-        <v>85</v>
-      </c>
-      <c r="P9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="D10" s="5">
         <v>0.3</v>
       </c>
       <c r="E10" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F10" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G10" t="s">
         <v>45</v>
@@ -1481,28 +2804,22 @@
       <c r="L10" t="s">
         <v>60</v>
       </c>
-      <c r="O10" t="s">
-        <v>86</v>
-      </c>
-      <c r="P10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="D11" s="5">
         <v>0.2</v>
       </c>
       <c r="E11" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F11" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G11" t="s">
         <v>45</v>
@@ -1519,14 +2836,8 @@
       <c r="M11" t="s">
         <v>58</v>
       </c>
-      <c r="O11" t="s">
-        <v>87</v>
-      </c>
-      <c r="P11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -1540,7 +2851,7 @@
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G12" t="s">
         <v>50</v>
@@ -1557,28 +2868,22 @@
       <c r="M12" t="s">
         <v>54</v>
       </c>
-      <c r="O12" t="s">
-        <v>88</v>
-      </c>
-      <c r="P12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D13" s="5">
         <v>0.1</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F13" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G13" t="s">
         <v>47</v>
@@ -1590,7 +2895,7 @@
         <v>69</v>
       </c>
       <c r="K13" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L13" t="s">
         <v>50</v>
@@ -1598,14 +2903,8 @@
       <c r="M13" t="s">
         <v>52</v>
       </c>
-      <c r="O13" t="s">
-        <v>89</v>
-      </c>
-      <c r="P13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -1616,10 +2915,10 @@
         <v>0.6</v>
       </c>
       <c r="E14" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F14" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G14" t="s">
         <v>50</v>
@@ -1639,48 +2938,36 @@
       <c r="M14" t="s">
         <v>56</v>
       </c>
-      <c r="O14" t="s">
-        <v>90</v>
-      </c>
-      <c r="P14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D15" s="5">
         <v>0.1</v>
       </c>
       <c r="E15" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F15" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G15" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="H15" t="s">
         <v>46</v>
       </c>
-      <c r="O15" t="s">
-        <v>91</v>
-      </c>
-      <c r="P15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D16" s="5">
         <v>1</v>
@@ -1689,7 +2976,7 @@
         <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G16" t="s">
         <v>53</v>
@@ -1697,34 +2984,28 @@
       <c r="H16" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="O16" t="s">
+      <c r="J16" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="P16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D17" s="5">
         <v>0.15</v>
       </c>
       <c r="E17" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F17" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G17" t="s">
         <v>72</v>
@@ -1744,28 +3025,22 @@
       <c r="M17" t="s">
         <v>5</v>
       </c>
-      <c r="O17" t="s">
-        <v>93</v>
-      </c>
-      <c r="P17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D18" s="5">
         <v>0.05</v>
       </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F18" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="G18" t="s">
         <v>47</v>
@@ -1774,7 +3049,7 @@
         <v>35</v>
       </c>
       <c r="K18" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="L18" t="s">
         <v>53</v>
@@ -1782,28 +3057,22 @@
       <c r="M18" t="s">
         <v>55</v>
       </c>
-      <c r="O18" t="s">
-        <v>94</v>
-      </c>
-      <c r="P18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="D19" s="5">
         <v>0.05</v>
       </c>
       <c r="E19" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F19" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G19" t="s">
         <v>48</v>
@@ -1812,10 +3081,10 @@
         <v>53</v>
       </c>
       <c r="J19" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="K19" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="L19" t="s">
         <v>45</v>
@@ -1823,122 +3092,100 @@
       <c r="M19" t="s">
         <v>56</v>
       </c>
-      <c r="O19" t="s">
-        <v>95</v>
-      </c>
-      <c r="P19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="5">
-        <v>1</v>
-      </c>
+      <c r="D20" s="5"/>
       <c r="E20" t="s">
         <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
       </c>
       <c r="K20" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="L20" t="s">
         <v>54</v>
       </c>
       <c r="M20" t="s">
-        <v>116</v>
-      </c>
-      <c r="O20" t="s">
-        <v>96</v>
-      </c>
-      <c r="P20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="5">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J21" t="s">
         <v>30</v>
       </c>
       <c r="K21" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="L21" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="M21" t="s">
         <v>45</v>
       </c>
-      <c r="O21" t="s">
-        <v>97</v>
-      </c>
-      <c r="P21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>165</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0.05</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="E22" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F22" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="J22" t="s">
         <v>31</v>
       </c>
       <c r="K22" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="L22" t="s">
         <v>54</v>
@@ -1947,62 +3194,62 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D23" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E23" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G23" t="s">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="H23" t="s">
+        <v>76</v>
       </c>
       <c r="J23" t="s">
         <v>32</v>
       </c>
       <c r="K23" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="L23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="D24" s="5">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E24" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F24" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="G24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J24" t="s">
         <v>28</v>
       </c>
       <c r="K24" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="L24" t="s">
         <v>57</v>
@@ -2011,24 +3258,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D25" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E25" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F25" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="G25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H25" t="s">
         <v>53</v>
@@ -2037,39 +3284,33 @@
         <v>27</v>
       </c>
       <c r="K25" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="L25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0.4</v>
+        <v>146</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J26" t="s">
         <v>37</v>
       </c>
       <c r="K26" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="L26" t="s">
         <v>46</v>
@@ -2078,33 +3319,33 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="D27" s="5">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="E27" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F27" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="G27" t="s">
         <v>47</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="J27" t="s">
         <v>59</v>
       </c>
       <c r="K27" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="L27" t="s">
         <v>50</v>
@@ -2113,62 +3354,63 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" t="s">
         <v>148</v>
       </c>
-      <c r="C28" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>161</v>
-      </c>
-      <c r="F28" t="s">
-        <v>160</v>
-      </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="H28" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J28" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="K28" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="L28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0.3</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="E29" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="H29" t="s">
+        <v>76</v>
       </c>
       <c r="J29" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="K29" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="L29" t="s">
         <v>57</v>
@@ -2177,33 +3419,31 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0.17</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D30" s="5"/>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="F30" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H30" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="J30" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="K30" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="L30" t="s">
         <v>58</v>
@@ -2212,65 +3452,68 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E31" t="s">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G31" t="s">
         <v>50</v>
       </c>
+      <c r="H31" t="s">
+        <v>53</v>
+      </c>
       <c r="J31" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="K31" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="L31" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="M31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D32" s="5">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="E32" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F32" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G32" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H32" t="s">
         <v>76</v>
       </c>
       <c r="J32" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="K32" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="L32" t="s">
         <v>57</v>
@@ -2281,28 +3524,31 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="D33" s="5">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
       <c r="E33" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F33" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G33" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="H33" t="s">
+        <v>58</v>
       </c>
       <c r="J33" t="s">
+        <v>85</v>
+      </c>
+      <c r="K33" t="s">
         <v>103</v>
-      </c>
-      <c r="K33" t="s">
-        <v>121</v>
       </c>
       <c r="L33" t="s">
         <v>60</v>
@@ -2310,66 +3556,63 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>172</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D34" s="5">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>149</v>
       </c>
       <c r="F34" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G34" t="s">
-        <v>126</v>
-      </c>
-      <c r="H34" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J34" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="K34" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="L34" t="s">
         <v>60</v>
       </c>
       <c r="M34" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="5">
-        <v>0.05</v>
+        <v>0.17</v>
       </c>
       <c r="E35" t="s">
-        <v>161</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G35" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H35" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J35" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="K35" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="L35" t="s">
         <v>51</v>
@@ -2377,28 +3620,28 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D36" s="5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E36" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="F36" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G36" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J36" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="K36" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="L36" t="s">
         <v>51</v>
@@ -2409,31 +3652,31 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D37" s="5">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F37" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G37" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="H37" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="J37" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="K37" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="L37" t="s">
         <v>48</v>
@@ -2444,31 +3687,28 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="D38" s="5">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="E38" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F38" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G38" t="s">
-        <v>45</v>
-      </c>
-      <c r="H38" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J38" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="K38" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="L38" t="s">
         <v>48</v>
@@ -2476,10 +3716,10 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>24</v>
+        <v>153</v>
       </c>
       <c r="C39" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="D39" s="5">
         <v>1</v>
@@ -2488,16 +3728,19 @@
         <v>79</v>
       </c>
       <c r="F39" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G39" t="s">
-        <v>54</v>
+        <v>108</v>
+      </c>
+      <c r="H39" t="s">
+        <v>47</v>
       </c>
       <c r="J39" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="K39" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="L39" t="s">
         <v>50</v>
@@ -2508,31 +3751,31 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>170</v>
+        <v>44</v>
       </c>
       <c r="D40" s="5">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F40" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H40" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J40" t="s">
         <v>41</v>
       </c>
       <c r="K40" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="L40" t="s">
         <v>47</v>
@@ -2543,39 +3786,39 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="D41" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F41" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G41" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J41" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="K41" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="L41" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>173</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D42" s="5">
         <v>1</v>
@@ -2584,44 +3827,56 @@
         <v>79</v>
       </c>
       <c r="F42" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G42" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="H42" t="s">
+        <v>53</v>
       </c>
       <c r="J42" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="K42" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="L42" t="s">
         <v>53</v>
       </c>
       <c r="M42" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>174</v>
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>140</v>
       </c>
       <c r="D43" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F43" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G43" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="H43" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>151</v>
       </c>
       <c r="D44" s="5">
         <v>1</v>
@@ -2630,325 +3885,319 @@
         <v>79</v>
       </c>
       <c r="F44" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G44" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>142</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D45" s="5">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F45" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G45" t="s">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="H45" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>143</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="D46" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F46" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G46" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C47" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="D47" s="5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F47" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G47" t="s">
-        <v>76</v>
-      </c>
-      <c r="H47" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
       <c r="D48" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F48" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="G48" t="s">
-        <v>47</v>
-      </c>
-      <c r="H48" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D49" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="F49" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G49" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D50" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>53</v>
+      <c r="B50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E50" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" t="s">
+        <v>141</v>
+      </c>
+      <c r="G50" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="D51" s="5">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="E51" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F51" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G51" t="s">
-        <v>56</v>
-      </c>
-      <c r="H51" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="D52" s="5">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E52" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F52" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G52" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="H52" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="D53" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E53" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F53" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="G53" t="s">
-        <v>116</v>
+        <v>47</v>
       </c>
       <c r="H53" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D54" s="5">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E54" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F54" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="G54" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" t="s">
-        <v>165</v>
-      </c>
-      <c r="D55" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="E55" t="s">
-        <v>161</v>
-      </c>
-      <c r="F55" t="s">
-        <v>160</v>
-      </c>
-      <c r="G55" t="s">
-        <v>58</v>
+      <c r="B55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D56" s="5">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E56" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F56" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G56" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+      <c r="H56" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>166</v>
+        <v>110</v>
       </c>
       <c r="D57" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E57" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F57" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G57" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="D58" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E58" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F58" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G58" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="H58" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="D59" s="5">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E59" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F59" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="G59" t="s">
         <v>76</v>
@@ -2956,128 +4205,122 @@
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>135</v>
+        <v>36</v>
       </c>
       <c r="C60" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="D60" s="5">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
       <c r="E60" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F60" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G60" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>136</v>
+        <v>38</v>
       </c>
       <c r="C61" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="D61" s="5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E61" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F61" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G61" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="C62" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="D62" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E62" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F62" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G62" t="s">
-        <v>57</v>
-      </c>
-      <c r="H62" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>138</v>
+        <v>39</v>
       </c>
       <c r="C63" t="s">
         <v>44</v>
       </c>
       <c r="D63" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E63" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F63" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G63" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H63" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D64" s="5">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E64" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F64" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="G64" t="s">
-        <v>60</v>
-      </c>
-      <c r="H64" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C65" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D65" s="5">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="E65" t="s">
-        <v>161</v>
-      </c>
-      <c r="F65" s="11" t="s">
-        <v>160</v>
+        <v>142</v>
+      </c>
+      <c r="F65" t="s">
+        <v>141</v>
       </c>
       <c r="G65" t="s">
         <v>72</v>
@@ -3085,44 +4328,350 @@
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="C66" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="D66" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E66" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F66" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G66" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C67" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D67" s="5">
         <v>0.1</v>
       </c>
       <c r="E67" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F67" t="s">
+        <v>141</v>
+      </c>
+      <c r="G67" t="s">
+        <v>57</v>
+      </c>
+      <c r="H67" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>142</v>
+      </c>
+      <c r="F68" t="s">
+        <v>141</v>
+      </c>
+      <c r="G68" t="s">
+        <v>53</v>
+      </c>
+      <c r="H68" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69" s="5">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>79</v>
+      </c>
+      <c r="F69" t="s">
+        <v>144</v>
+      </c>
+      <c r="G69" t="s">
+        <v>60</v>
+      </c>
+      <c r="H69" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="E70" t="s">
+        <v>142</v>
+      </c>
+      <c r="F70" t="s">
+        <v>141</v>
+      </c>
+      <c r="G70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D71" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E71" t="s">
+        <v>142</v>
+      </c>
+      <c r="F71" t="s">
+        <v>141</v>
+      </c>
+      <c r="G71" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>114</v>
+      </c>
+      <c r="C72" t="s">
+        <v>110</v>
+      </c>
+      <c r="D72" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>142</v>
+      </c>
+      <c r="F72" t="s">
+        <v>144</v>
+      </c>
+      <c r="G72" t="s">
+        <v>47</v>
+      </c>
+      <c r="H72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>163</v>
       </c>
-      <c r="G67" t="s">
-        <v>47</v>
-      </c>
-      <c r="H67" t="s">
+      <c r="C73" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" t="s">
+        <v>79</v>
+      </c>
+      <c r="F73" t="s">
+        <v>141</v>
+      </c>
+      <c r="G73" t="s">
+        <v>48</v>
+      </c>
+      <c r="H73" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" t="s">
+        <v>164</v>
+      </c>
+      <c r="E74" t="s">
+        <v>79</v>
+      </c>
+      <c r="F74" t="s">
+        <v>141</v>
+      </c>
+      <c r="G74" t="s">
+        <v>98</v>
+      </c>
+      <c r="H74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>166</v>
+      </c>
+      <c r="C75" t="s">
+        <v>164</v>
+      </c>
+      <c r="E75" t="s">
+        <v>79</v>
+      </c>
+      <c r="F75" t="s">
+        <v>141</v>
+      </c>
+      <c r="G75" t="s">
+        <v>98</v>
+      </c>
+      <c r="H75" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>167</v>
+      </c>
+      <c r="C76" t="s">
+        <v>164</v>
+      </c>
+      <c r="E76" t="s">
+        <v>79</v>
+      </c>
+      <c r="F76" t="s">
+        <v>141</v>
+      </c>
+      <c r="G76" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>168</v>
+      </c>
+      <c r="C77" t="s">
+        <v>164</v>
+      </c>
+      <c r="E77" t="s">
+        <v>79</v>
+      </c>
+      <c r="F77" t="s">
+        <v>141</v>
+      </c>
+      <c r="G77" t="s">
+        <v>51</v>
+      </c>
+      <c r="H77" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" t="s">
+        <v>164</v>
+      </c>
+      <c r="E78" t="s">
+        <v>79</v>
+      </c>
+      <c r="F78" t="s">
+        <v>141</v>
+      </c>
+      <c r="G78" t="s">
+        <v>54</v>
+      </c>
+      <c r="H78" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>170</v>
+      </c>
+      <c r="C79" t="s">
+        <v>164</v>
+      </c>
+      <c r="E79" t="s">
+        <v>79</v>
+      </c>
+      <c r="F79" t="s">
+        <v>141</v>
+      </c>
+      <c r="G79" t="s">
+        <v>53</v>
+      </c>
+      <c r="H79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" t="s">
+        <v>164</v>
+      </c>
+      <c r="E80" t="s">
+        <v>79</v>
+      </c>
+      <c r="F80" t="s">
+        <v>141</v>
+      </c>
+      <c r="G80" t="s">
+        <v>45</v>
+      </c>
+      <c r="H80" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>172</v>
+      </c>
+      <c r="C81" t="s">
+        <v>164</v>
+      </c>
+      <c r="E81" t="s">
+        <v>79</v>
+      </c>
+      <c r="F81" t="s">
+        <v>141</v>
+      </c>
+      <c r="G81" t="s">
+        <v>48</v>
+      </c>
+      <c r="H81" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>173</v>
+      </c>
+      <c r="C82" t="s">
+        <v>164</v>
+      </c>
+      <c r="E82" t="s">
+        <v>79</v>
+      </c>
+      <c r="F82" t="s">
+        <v>141</v>
+      </c>
+      <c r="G82" t="s">
+        <v>56</v>
+      </c>
+      <c r="H82" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3135,11 +4684,236 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09E350B-F8D3-4669-88FA-2F725652E15C}">
+  <dimension ref="B1:M22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="21"/>
+    </row>
+    <row r="2" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>